<commit_message>
ajustes en esacaleta 07-13
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion13/Escaleta_CN_07_13_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion13/Escaleta_CN_07_13_CO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mpgarcia\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado07\guion13\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -438,9 +443,6 @@
     <t>Los descubrimientos biológicos que cambiaron para siempre la medicina</t>
   </si>
   <si>
-    <t xml:space="preserve">Las sanguijuelas en la medicina actual </t>
-  </si>
-  <si>
     <t>El descubrimiento de los microbios y su relación con las enfermedades</t>
   </si>
   <si>
@@ -724,6 +726,9 @@
   </si>
   <si>
     <t>Interactivo para ordenar los pasos en el proceso de elaboración de un test químico</t>
+  </si>
+  <si>
+    <t>¿Qué son las sanguijuelas?</t>
   </si>
 </sst>
 </file>
@@ -963,34 +968,20 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1032,9 +1023,23 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1096,7 +1101,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1131,7 +1136,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1343,9 +1348,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:U285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V30" sqref="V30"/>
+      <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,94 +1378,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="30" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="I1" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="55" t="s">
+      <c r="M1" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="35" t="s">
+      <c r="N1" s="51"/>
+      <c r="O1" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="Q1" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="41" t="s">
+      <c r="R1" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="37" t="s">
+      <c r="S1" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="T1" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="37" t="s">
+      <c r="U1" s="54" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="30" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="50"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="46"/>
       <c r="M2" s="31" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="42"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="38"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="55"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
@@ -1545,7 +1550,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>20</v>
@@ -1604,7 +1609,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1654,16 +1659,16 @@
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="16" t="s">
-        <v>139</v>
+        <v>234</v>
       </c>
       <c r="H7" s="9">
         <v>3</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>20</v>
@@ -1683,13 +1688,13 @@
         <v>6</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S7" s="10" t="s">
         <v>129</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="U7" s="10" t="s">
         <v>131</v>
@@ -1712,10 +1717,10 @@
         <v>138</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G8" s="16" t="s">
         <v>140</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>141</v>
       </c>
       <c r="H8" s="9">
         <v>4</v>
@@ -1724,7 +1729,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>19</v>
@@ -1741,19 +1746,19 @@
         <v>19</v>
       </c>
       <c r="Q8" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="R8" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="R8" s="11" t="s">
+      <c r="S8" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="S8" s="10" t="s">
+      <c r="T8" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="U8" s="10" t="s">
         <v>144</v>
-      </c>
-      <c r="T8" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="U8" s="10" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1773,10 +1778,10 @@
         <v>138</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H9" s="9">
         <v>5</v>
@@ -1785,7 +1790,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>20</v>
@@ -1811,7 +1816,7 @@
         <v>135</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="U9" s="10" t="s">
         <v>137</v>
@@ -1834,10 +1839,10 @@
         <v>138</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H10" s="9">
         <v>6</v>
@@ -1846,7 +1851,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>20</v>
@@ -1872,7 +1877,7 @@
         <v>135</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="U10" s="10" t="s">
         <v>137</v>
@@ -1896,7 +1901,7 @@
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H11" s="9">
         <v>7</v>
@@ -1905,7 +1910,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>20</v>
@@ -1931,7 +1936,7 @@
         <v>135</v>
       </c>
       <c r="T11" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="U11" s="10" t="s">
         <v>137</v>
@@ -1948,12 +1953,12 @@
         <v>124</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="9"/>
       <c r="G12" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H12" s="9">
         <v>8</v>
@@ -1962,7 +1967,7 @@
         <v>19</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>20</v>
@@ -1982,13 +1987,13 @@
         <v>6</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S12" s="10" t="s">
         <v>129</v>
       </c>
       <c r="T12" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="U12" s="10" t="s">
         <v>131</v>
@@ -2005,14 +2010,14 @@
         <v>124</v>
       </c>
       <c r="D13" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>153</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>154</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H13" s="9">
         <v>9</v>
@@ -2021,7 +2026,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>20</v>
@@ -2047,7 +2052,7 @@
         <v>135</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U13" s="10" t="s">
         <v>137</v>
@@ -2064,14 +2069,14 @@
         <v>124</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H14" s="9">
         <v>10</v>
@@ -2080,7 +2085,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>20</v>
@@ -2106,7 +2111,7 @@
         <v>135</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="U14" s="10" t="s">
         <v>137</v>
@@ -2123,14 +2128,14 @@
         <v>124</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H15" s="9">
         <v>11</v>
@@ -2139,7 +2144,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2159,13 +2164,13 @@
         <v>6</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S15" s="10" t="s">
         <v>129</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="U15" s="10" t="s">
         <v>131</v>
@@ -2182,14 +2187,14 @@
         <v>124</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>132</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H16" s="9">
         <v>12</v>
@@ -2198,7 +2203,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>20</v>
@@ -2224,7 +2229,7 @@
         <v>135</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="U16" s="10" t="s">
         <v>137</v>
@@ -2241,14 +2246,14 @@
         <v>124</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H17" s="9">
         <v>13</v>
@@ -2257,7 +2262,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>20</v>
@@ -2277,13 +2282,13 @@
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S17" s="10" t="s">
         <v>129</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="U17" s="10" t="s">
         <v>131</v>
@@ -2300,14 +2305,14 @@
         <v>124</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H18" s="9">
         <v>14</v>
@@ -2316,7 +2321,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2342,7 +2347,7 @@
         <v>135</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="U18" s="10" t="s">
         <v>137</v>
@@ -2359,14 +2364,14 @@
         <v>124</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>132</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H19" s="9">
         <v>15</v>
@@ -2375,7 +2380,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2401,7 +2406,7 @@
         <v>135</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U19" s="10" t="s">
         <v>137</v>
@@ -2418,25 +2423,25 @@
         <v>124</v>
       </c>
       <c r="D20" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="F20" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>178</v>
-      </c>
       <c r="G20" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H20" s="9">
         <v>16</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>20</v>
@@ -2459,13 +2464,13 @@
         <v>134</v>
       </c>
       <c r="S20" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="T20" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="T20" s="12" t="s">
+      <c r="U20" s="10" t="s">
         <v>198</v>
-      </c>
-      <c r="U20" s="10" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2479,16 +2484,16 @@
         <v>124</v>
       </c>
       <c r="D21" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>177</v>
-      </c>
       <c r="F21" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H21" s="9">
         <v>17</v>
@@ -2497,7 +2502,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>20</v>
@@ -2523,7 +2528,7 @@
         <v>135</v>
       </c>
       <c r="T21" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="U21" s="10" t="s">
         <v>137</v>
@@ -2540,14 +2545,14 @@
         <v>124</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H22" s="9">
         <v>18</v>
@@ -2556,7 +2561,7 @@
         <v>19</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>20</v>
@@ -2576,13 +2581,13 @@
         <v>6</v>
       </c>
       <c r="R22" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S22" s="10" t="s">
         <v>129</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="U22" s="10" t="s">
         <v>131</v>
@@ -2599,14 +2604,14 @@
         <v>124</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>132</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H23" s="9">
         <v>19</v>
@@ -2615,7 +2620,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>20</v>
@@ -2641,7 +2646,7 @@
         <v>135</v>
       </c>
       <c r="T23" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="U23" s="10" t="s">
         <v>137</v>
@@ -2658,12 +2663,12 @@
         <v>124</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="9"/>
       <c r="G24" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H24" s="9">
         <v>20</v>
@@ -2672,7 +2677,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>20</v>
@@ -2698,7 +2703,7 @@
         <v>135</v>
       </c>
       <c r="T24" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U24" s="10" t="s">
         <v>137</v>
@@ -2715,12 +2720,12 @@
         <v>124</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="9"/>
       <c r="G25" s="16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H25" s="9">
         <v>21</v>
@@ -2729,7 +2734,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>20</v>
@@ -2755,7 +2760,7 @@
         <v>135</v>
       </c>
       <c r="T25" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="U25" s="10" t="s">
         <v>137</v>
@@ -2772,12 +2777,12 @@
         <v>124</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="9"/>
       <c r="G26" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H26" s="9">
         <v>22</v>
@@ -2786,7 +2791,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>20</v>
@@ -2812,7 +2817,7 @@
         <v>135</v>
       </c>
       <c r="T26" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U26" s="10" t="s">
         <v>137</v>
@@ -2829,12 +2834,12 @@
         <v>124</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E27" s="13"/>
       <c r="F27" s="9"/>
       <c r="G27" s="16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H27" s="9">
         <v>23</v>
@@ -2843,7 +2848,7 @@
         <v>19</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>20</v>
@@ -2863,13 +2868,13 @@
         <v>6</v>
       </c>
       <c r="R27" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S27" s="10" t="s">
         <v>129</v>
       </c>
       <c r="T27" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="U27" s="10" t="s">
         <v>131</v>
@@ -2886,12 +2891,12 @@
         <v>124</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="9"/>
       <c r="G28" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H28" s="9">
         <v>24</v>
@@ -2900,7 +2905,7 @@
         <v>19</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>20</v>
@@ -2920,13 +2925,13 @@
         <v>6</v>
       </c>
       <c r="R28" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S28" s="10" t="s">
         <v>129</v>
       </c>
       <c r="T28" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U28" s="10" t="s">
         <v>131</v>
@@ -2943,12 +2948,12 @@
         <v>124</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="9"/>
       <c r="G29" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H29" s="9">
         <v>25</v>
@@ -2957,7 +2962,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>20</v>
@@ -2983,7 +2988,7 @@
         <v>135</v>
       </c>
       <c r="T29" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="U29" s="10" t="s">
         <v>137</v>
@@ -3000,7 +3005,7 @@
         <v>124</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="9"/>
@@ -3014,7 +3019,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>20</v>
@@ -3043,12 +3048,12 @@
         <v>124</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="9"/>
       <c r="G31" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H31" s="9">
         <v>27</v>
@@ -3057,7 +3062,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>20</v>
@@ -3083,7 +3088,7 @@
         <v>135</v>
       </c>
       <c r="T31" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U31" s="10" t="s">
         <v>137</v>
@@ -3091,13 +3096,13 @@
     </row>
     <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="58"/>
+      <c r="B32" s="35"/>
       <c r="C32" s="14"/>
       <c r="D32" s="15"/>
       <c r="E32" s="13"/>
       <c r="F32" s="9"/>
       <c r="G32" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H32" s="9">
         <v>28</v>
@@ -3106,7 +3111,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>20</v>
@@ -3170,7 +3175,7 @@
         <v>124</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E34" s="13"/>
       <c r="F34" s="9"/>
@@ -3201,7 +3206,7 @@
         <v>124</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E35" s="13"/>
       <c r="F35" s="9"/>
@@ -3232,10 +3237,10 @@
         <v>124</v>
       </c>
       <c r="D36" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="E36" s="13" t="s">
         <v>166</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>167</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="16"/>
@@ -3265,7 +3270,7 @@
         <v>124</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E37" s="13"/>
       <c r="F37" s="9"/>
@@ -3289,17 +3294,17 @@
       <c r="A38" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="59" t="s">
+      <c r="B38" s="36" t="s">
         <v>122</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>124</v>
       </c>
       <c r="D38" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="E38" s="13" t="s">
         <v>176</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>177</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="16"/>
@@ -4449,6 +4454,12 @@
     </sortState>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4463,12 +4474,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>